<commit_message>
refactor a lot and changed the folders structure
</commit_message>
<xml_diff>
--- a/test-iot-datasets.xlsx
+++ b/test-iot-datasets.xlsx
@@ -5,25 +5,35 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/efraim_efraimpartoginahotasi_wur_nl/Documents/2. Thesis - Information Technology/3. Software Projects/calibrator-model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frm19\OneDrive - Wageningen University &amp; Research\2. Thesis - Information Technology\3. Software Projects\mini-greenhouse-calibrator-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_7129F58C5B80D716477B3411595ED87656CD7D53" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8E09707-BA54-4C57-B4D5-16C352AD28E8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBFD8AD1-C990-4A5A-9214-DBAF302E8779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1910" yWindow="-10500" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>global out</t>
-  </si>
   <si>
     <t>global in</t>
   </si>
@@ -56,6 +66,9 @@
   </si>
   <si>
     <t>time</t>
+  </si>
+  <si>
+    <t>global out</t>
   </si>
 </sst>
 </file>
@@ -421,52 +434,52 @@
   <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>0</v>
+        <v>1200</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -504,7 +517,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>300</v>
+        <v>1500</v>
       </c>
       <c r="B3">
         <v>2.9624999999999999E-2</v>
@@ -542,7 +555,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>600</v>
+        <v>1800</v>
       </c>
       <c r="B4">
         <v>3.2943E-2</v>
@@ -580,7 +593,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>900</v>
+        <v>2100</v>
       </c>
       <c r="B5">
         <v>3.2943E-2</v>
@@ -618,7 +631,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>1200</v>
+        <v>2400</v>
       </c>
       <c r="B6">
         <v>1.0980999999999999E-2</v>
@@ -656,7 +669,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>1500</v>
+        <v>2700</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -694,7 +707,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>1800</v>
+        <v>3000</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -732,7 +745,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>2100</v>
+        <v>3300</v>
       </c>
       <c r="B9">
         <v>2.1961999999999999E-2</v>
@@ -770,7 +783,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>2400</v>
+        <v>3600</v>
       </c>
       <c r="B10">
         <v>2.9624999999999999E-2</v>
@@ -808,7 +821,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>2700</v>
+        <v>3900</v>
       </c>
       <c r="B11">
         <v>2.8518999999999999E-2</v>
@@ -846,7 +859,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>3000</v>
+        <v>4200</v>
       </c>
       <c r="B12">
         <v>3.2943E-2</v>
@@ -884,7 +897,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>3300</v>
+        <v>4500</v>
       </c>
       <c r="B13">
         <v>3.2943E-2</v>
@@ -922,7 +935,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>3600</v>
+        <v>1200</v>
       </c>
       <c r="B14">
         <v>21.211500000000001</v>
@@ -960,7 +973,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>3900</v>
+        <v>1500</v>
       </c>
       <c r="B15">
         <v>21.0535</v>
@@ -998,7 +1011,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>4200</v>
+        <v>1800</v>
       </c>
       <c r="B16">
         <v>20.168700000000001</v>
@@ -1036,7 +1049,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>4500</v>
+        <v>2100</v>
       </c>
       <c r="B17">
         <v>19.694700000000001</v>
@@ -1074,7 +1087,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>4800</v>
+        <v>2400</v>
       </c>
       <c r="B18">
         <v>19.386600000000001</v>
@@ -1112,7 +1125,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>5100</v>
+        <v>2700</v>
       </c>
       <c r="B19">
         <v>19.1812</v>
@@ -1150,7 +1163,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>5400</v>
+        <v>3000</v>
       </c>
       <c r="B20">
         <v>18.462299999999999</v>
@@ -1188,7 +1201,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>5700</v>
+        <v>3300</v>
       </c>
       <c r="B21">
         <v>18.612400000000001</v>
@@ -1226,7 +1239,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>6000</v>
+        <v>3600</v>
       </c>
       <c r="B22">
         <v>17.696000000000002</v>
@@ -1264,7 +1277,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>6300</v>
+        <v>3900</v>
       </c>
       <c r="B23">
         <v>17.8066</v>
@@ -1302,7 +1315,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>6600</v>
+        <v>4200</v>
       </c>
       <c r="B24">
         <v>19.2286</v>
@@ -1340,7 +1353,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>6900</v>
+        <v>4500</v>
       </c>
       <c r="B25">
         <v>18.572900000000001</v>
@@ -1378,7 +1391,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>7200</v>
+        <v>1200</v>
       </c>
       <c r="B26">
         <v>14.085699999999999</v>
@@ -1416,7 +1429,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>7500</v>
+        <v>1500</v>
       </c>
       <c r="B27">
         <v>13.587999999999999</v>
@@ -1454,7 +1467,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>7800</v>
+        <v>1800</v>
       </c>
       <c r="B28">
         <v>13.461600000000001</v>
@@ -1492,7 +1505,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>8100</v>
+        <v>2100</v>
       </c>
       <c r="B29">
         <v>12.529400000000001</v>
@@ -1530,7 +1543,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>8400</v>
+        <v>2400</v>
       </c>
       <c r="B30">
         <v>12.2371</v>
@@ -1568,7 +1581,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31">
-        <v>8700</v>
+        <v>2700</v>
       </c>
       <c r="B31">
         <v>11.692</v>
@@ -1606,7 +1619,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>9000</v>
+        <v>3000</v>
       </c>
       <c r="B32">
         <v>11.249599999999999</v>
@@ -1644,7 +1657,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33">
-        <v>9300</v>
+        <v>3300</v>
       </c>
       <c r="B33">
         <v>10.973100000000001</v>
@@ -1682,7 +1695,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34">
-        <v>9600</v>
+        <v>3600</v>
       </c>
       <c r="B34">
         <v>10.293699999999999</v>
@@ -1720,7 +1733,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35">
-        <v>9900</v>
+        <v>3900</v>
       </c>
       <c r="B35">
         <v>9.6301000000000005</v>
@@ -1758,7 +1771,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36">
-        <v>10200</v>
+        <v>4200</v>
       </c>
       <c r="B36">
         <v>9.3694000000000006</v>
@@ -1796,7 +1809,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37">
-        <v>10500</v>
+        <v>4500</v>
       </c>
       <c r="B37">
         <v>8.8559000000000001</v>
@@ -1834,7 +1847,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38">
-        <v>10800</v>
+        <v>4800</v>
       </c>
       <c r="B38">
         <v>8.4372000000000007</v>
@@ -1872,7 +1885,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39">
-        <v>11100</v>
+        <v>5100</v>
       </c>
       <c r="B39">
         <v>8.3187000000000015</v>
@@ -1910,7 +1923,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40">
-        <v>11400</v>
+        <v>5400</v>
       </c>
       <c r="B40">
         <v>8.4688000000000017</v>
@@ -1948,7 +1961,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41">
-        <v>11700</v>
+        <v>5700</v>
       </c>
       <c r="B41">
         <v>8.6110000000000007</v>
@@ -1986,7 +1999,7 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42">
-        <v>12000</v>
+        <v>6000</v>
       </c>
       <c r="B42">
         <v>8.7611000000000008</v>
@@ -2024,7 +2037,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43">
-        <v>12300</v>
+        <v>6300</v>
       </c>
       <c r="B43">
         <v>8.476700000000001</v>
@@ -2062,7 +2075,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44">
-        <v>12600</v>
+        <v>6600</v>
       </c>
       <c r="B44">
         <v>7.9316000000000004</v>
@@ -2100,7 +2113,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45">
-        <v>12900</v>
+        <v>6900</v>
       </c>
       <c r="B45">
         <v>7.7499000000000011</v>
@@ -2138,7 +2151,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46">
-        <v>13200</v>
+        <v>7200</v>
       </c>
       <c r="B46">
         <v>8.1449000000000016</v>
@@ -2176,7 +2189,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47">
-        <v>13500</v>
+        <v>7500</v>
       </c>
       <c r="B47">
         <v>8.2871000000000006</v>
@@ -2214,7 +2227,7 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48">
-        <v>13800</v>
+        <v>7800</v>
       </c>
       <c r="B48">
         <v>8.0106000000000002</v>
@@ -2252,7 +2265,7 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49">
-        <v>14100</v>
+        <v>8100</v>
       </c>
       <c r="B49">
         <v>7.7894000000000014</v>
@@ -2290,7 +2303,7 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50">
-        <v>14400</v>
+        <v>1200</v>
       </c>
       <c r="B50">
         <v>3.4839000000000002</v>
@@ -2328,7 +2341,7 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51">
-        <v>14700</v>
+        <v>1500</v>
       </c>
       <c r="B51">
         <v>3.3891</v>
@@ -2366,7 +2379,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52">
-        <v>15000</v>
+        <v>1800</v>
       </c>
       <c r="B52">
         <v>3.436500000000001</v>
@@ -2404,7 +2417,7 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53">
-        <v>15300</v>
+        <v>2100</v>
       </c>
       <c r="B53">
         <v>3.333800000000001</v>
@@ -2442,7 +2455,7 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54">
-        <v>15600</v>
+        <v>2400</v>
       </c>
       <c r="B54">
         <v>3.231100000000001</v>
@@ -2480,7 +2493,7 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55">
-        <v>15900</v>
+        <v>2700</v>
       </c>
       <c r="B55">
         <v>3.1362999999999999</v>
@@ -2518,7 +2531,7 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56">
-        <v>16200</v>
+        <v>3000</v>
       </c>
       <c r="B56">
         <v>3.1126</v>
@@ -2556,7 +2569,7 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57">
-        <v>16500</v>
+        <v>3300</v>
       </c>
       <c r="B57">
         <v>3.0019999999999998</v>
@@ -2594,7 +2607,7 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58">
-        <v>16800</v>
+        <v>3600</v>
       </c>
       <c r="B58">
         <v>2.8835000000000002</v>
@@ -2632,7 +2645,7 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59">
-        <v>17100</v>
+        <v>3900</v>
       </c>
       <c r="B59">
         <v>2.8519000000000001</v>
@@ -2670,7 +2683,7 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60">
-        <v>17400</v>
+        <v>4200</v>
       </c>
       <c r="B60">
         <v>2.7492000000000001</v>
@@ -2708,7 +2721,7 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61">
-        <v>17700</v>
+        <v>4500</v>
       </c>
       <c r="B61">
         <v>2.5912000000000002</v>

</xml_diff>